<commit_message>
Update output files. (Some new files, some path updates. Just mass update.)
</commit_message>
<xml_diff>
--- a/processing_files/excel/schedule-lists_owners-grouped.xlsx
+++ b/processing_files/excel/schedule-lists_owners-grouped.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="teachers" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="classrooms" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="subjects" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="classes" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="teachers" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="classrooms" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="subjects" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -470,6 +471,499 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
+  <dimension ref="A1:F24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="11" customWidth="1" min="2" max="2"/>
+    <col width="12" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="13" customWidth="1" min="5" max="5"/>
+    <col width="11" customWidth="1" min="6" max="6"/>
+  </cols>
+  <sheetData>
+    <row r="1"/>
+    <row r="2" ht="14.3" customHeight="1">
+      <c r="A2" s="1" t="n"/>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>group_No.</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>names_base</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>names_in_group_No.</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>names</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>names_No.</t>
+        </is>
+      </c>
+    </row>
+    <row r="3" ht="14.3" customHeight="1">
+      <c r="A3" s="1" t="n"/>
+      <c r="B3" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="C3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E3" s="4" t="inlineStr">
+        <is>
+          <t>1B 1gas_log</t>
+        </is>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" ht="14.3" customHeight="1">
+      <c r="A4" s="1" t="n"/>
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>1d 1wz</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" ht="14.3" customHeight="1">
+      <c r="A5" s="1" t="n"/>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E5" s="1" t="inlineStr">
+        <is>
+          <t>2A 2ek_fry</t>
+        </is>
+      </c>
+      <c r="F5" s="1" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" ht="14.3" customHeight="1">
+      <c r="A6" s="1" t="n"/>
+      <c r="B6" s="2" t="n"/>
+      <c r="C6" s="2" t="n"/>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E6" s="1" t="inlineStr">
+        <is>
+          <t>2B 2gas</t>
+        </is>
+      </c>
+      <c r="F6" s="1" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" ht="14.3" customHeight="1">
+      <c r="A7" s="1" t="n"/>
+      <c r="B7" s="2" t="n"/>
+      <c r="C7" s="2" t="n"/>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="E7" s="1" t="inlineStr">
+        <is>
+          <t>2C 2hot</t>
+        </is>
+      </c>
+      <c r="F7" s="1" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" ht="14.3" customHeight="1">
+      <c r="A8" s="1" t="n"/>
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="E8" s="1" t="inlineStr">
+        <is>
+          <t>2L 2log</t>
+        </is>
+      </c>
+      <c r="F8" s="1" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" ht="14.3" customHeight="1">
+      <c r="A9" s="1" t="n"/>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="inlineStr">
+        <is>
+          <t>2d 2wz</t>
+        </is>
+      </c>
+      <c r="F9" s="1" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" ht="14.3" customHeight="1">
+      <c r="A10" s="1" t="n"/>
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>3</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="inlineStr">
+        <is>
+          <t>3A 3ra_fry</t>
+        </is>
+      </c>
+      <c r="F10" s="4" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" ht="14.3" customHeight="1">
+      <c r="A11" s="1" t="n"/>
+      <c r="B11" s="3" t="n"/>
+      <c r="C11" s="3" t="n"/>
+      <c r="D11" s="3" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E11" s="4" t="inlineStr">
+        <is>
+          <t>3B 3gas</t>
+        </is>
+      </c>
+      <c r="F11" s="4" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" ht="14.3" customHeight="1">
+      <c r="A12" s="1" t="n"/>
+      <c r="B12" s="3" t="n"/>
+      <c r="C12" s="3" t="n"/>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="inlineStr">
+        <is>
+          <t>3C 3hot</t>
+        </is>
+      </c>
+      <c r="F12" s="4" t="n">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" ht="14.3" customHeight="1">
+      <c r="A13" s="1" t="n"/>
+      <c r="B13" s="3" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="inlineStr">
+        <is>
+          <t>3JL</t>
+        </is>
+      </c>
+      <c r="F13" s="4" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" ht="14.3" customHeight="1">
+      <c r="A14" s="1" t="n"/>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
+      <c r="D14" s="3" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="E14" s="4" t="inlineStr">
+        <is>
+          <t>3L 3log</t>
+        </is>
+      </c>
+      <c r="F14" s="4" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" ht="14.3" customHeight="1">
+      <c r="A15" s="1" t="n"/>
+      <c r="B15" s="3" t="n"/>
+      <c r="C15" s="3" t="n"/>
+      <c r="D15" s="3" t="inlineStr">
+        <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="E15" s="4" t="inlineStr">
+        <is>
+          <t>3S 3sport</t>
+        </is>
+      </c>
+      <c r="F15" s="4" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" ht="14.3" customHeight="1">
+      <c r="A16" s="1" t="n"/>
+      <c r="B16" s="3" t="n"/>
+      <c r="C16" s="3" t="n"/>
+      <c r="D16" s="3" t="inlineStr">
+        <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="E16" s="4" t="inlineStr">
+        <is>
+          <t>3d 3wz</t>
+        </is>
+      </c>
+      <c r="F16" s="4" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" ht="14.3" customHeight="1">
+      <c r="A17" s="1" t="n"/>
+      <c r="B17" s="3" t="n"/>
+      <c r="C17" s="3" t="n"/>
+      <c r="D17" s="3" t="inlineStr">
+        <is>
+          <t>8.</t>
+        </is>
+      </c>
+      <c r="E17" s="4" t="inlineStr">
+        <is>
+          <t>3e 3wz</t>
+        </is>
+      </c>
+      <c r="F17" s="4" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" ht="14.3" customHeight="1">
+      <c r="A18" s="1" t="n"/>
+      <c r="B18" s="2" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="C18" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" s="2" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E18" s="1" t="inlineStr">
+        <is>
+          <t>4A 4ra_log</t>
+        </is>
+      </c>
+      <c r="F18" s="1" t="n">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" ht="14.3" customHeight="1">
+      <c r="A19" s="1" t="n"/>
+      <c r="B19" s="2" t="n"/>
+      <c r="C19" s="2" t="n"/>
+      <c r="D19" s="2" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E19" s="1" t="inlineStr">
+        <is>
+          <t>4B 4gas_fry</t>
+        </is>
+      </c>
+      <c r="F19" s="1" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" ht="14.3" customHeight="1">
+      <c r="A20" s="1" t="n"/>
+      <c r="B20" s="3" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="C20" s="3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E20" s="4" t="inlineStr">
+        <is>
+          <t>5A 5ek_log</t>
+        </is>
+      </c>
+      <c r="F20" s="4" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" ht="14.3" customHeight="1">
+      <c r="A21" s="1" t="n"/>
+      <c r="B21" s="3" t="n"/>
+      <c r="C21" s="3" t="n"/>
+      <c r="D21" s="3" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E21" s="4" t="inlineStr">
+        <is>
+          <t>5B 5gas_fry</t>
+        </is>
+      </c>
+      <c r="F21" s="4" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" ht="14.3" customHeight="1">
+      <c r="A22" s="1" t="n"/>
+      <c r="B22" s="3" t="n"/>
+      <c r="C22" s="3" t="n"/>
+      <c r="D22" s="3" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="E22" s="4" t="inlineStr">
+        <is>
+          <t>5MP</t>
+        </is>
+      </c>
+      <c r="F22" s="4" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" ht="14.3" customHeight="1">
+      <c r="A23" s="1" t="n"/>
+      <c r="B23" s="3" t="n"/>
+      <c r="C23" s="3" t="n"/>
+      <c r="D23" s="3" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="E23" s="4" t="inlineStr">
+        <is>
+          <t>5OP</t>
+        </is>
+      </c>
+      <c r="F23" s="4" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" ht="14.3" customHeight="1">
+      <c r="A24" s="1" t="n"/>
+      <c r="B24" s="3" t="n"/>
+      <c r="C24" s="3" t="n"/>
+      <c r="D24" s="3" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="E24" s="4" t="inlineStr">
+        <is>
+          <t>5ZI</t>
+        </is>
+      </c>
+      <c r="F24" s="4" t="n">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="C10:C17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C20:C24"/>
+    <mergeCell ref="B20:B24"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="B10:B17"/>
+    <mergeCell ref="B5:B9"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:F47"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1473,7 +1967,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2132,7 +2626,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>

</xml_diff>

<commit_message>
Update Excel output files.
</commit_message>
<xml_diff>
--- a/processing_files/excel/schedule-lists_owners-grouped.xlsx
+++ b/processing_files/excel/schedule-lists_owners-grouped.xlsx
@@ -477,7 +477,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -970,7 +970,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -1979,7 +1979,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="12" customWidth="1" min="3" max="3"/>
@@ -2638,7 +2638,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="11" customWidth="1" min="2" max="2"/>
     <col width="13" customWidth="1" min="3" max="3"/>

</xml_diff>

<commit_message>
Update output file names and content.
</commit_message>
<xml_diff>
--- a/processing_files/excel/schedule-lists_owners-grouped.xlsx
+++ b/processing_files/excel/schedule-lists_owners-grouped.xlsx
@@ -468,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -521,7 +521,7 @@
       </c>
       <c r="C3" s="3" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>sg</t>
         </is>
       </c>
       <c r="D3" s="3" t="inlineStr">
@@ -531,7 +531,7 @@
       </c>
       <c r="E3" s="4" t="inlineStr">
         <is>
-          <t>B</t>
+          <t>sg1</t>
         </is>
       </c>
       <c r="F3" s="4" t="n">
@@ -540,131 +540,107 @@
     </row>
     <row r="4" ht="14.3" customHeight="1">
       <c r="A4" s="1" t="n"/>
-      <c r="B4" s="2" t="inlineStr">
+      <c r="B4" s="3" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="inlineStr">
         <is>
           <t>2.</t>
         </is>
       </c>
-      <c r="C4" s="2" t="inlineStr">
-        <is>
-          <t>s</t>
-        </is>
-      </c>
-      <c r="D4" s="2" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="E4" s="1" t="inlineStr">
-        <is>
-          <t>s1</t>
-        </is>
-      </c>
-      <c r="F4" s="1" t="n">
+      <c r="E4" s="4" t="inlineStr">
+        <is>
+          <t>sg2</t>
+        </is>
+      </c>
+      <c r="F4" s="4" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="5" ht="14.3" customHeight="1">
       <c r="A5" s="1" t="n"/>
-      <c r="B5" s="2" t="n"/>
-      <c r="C5" s="2" t="n"/>
-      <c r="D5" s="2" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="E5" s="1" t="inlineStr">
-        <is>
-          <t>s2</t>
-        </is>
-      </c>
-      <c r="F5" s="1" t="n">
+      <c r="B5" s="3" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="E5" s="4" t="inlineStr">
+        <is>
+          <t>sg3</t>
+        </is>
+      </c>
+      <c r="F5" s="4" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="6" ht="14.3" customHeight="1">
       <c r="A6" s="1" t="n"/>
-      <c r="B6" s="2" t="n"/>
-      <c r="C6" s="2" t="n"/>
-      <c r="D6" s="2" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="E6" s="1" t="inlineStr">
-        <is>
-          <t>s3</t>
-        </is>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="B6" s="3" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="E6" s="4" t="inlineStr">
+        <is>
+          <t>sg4</t>
+        </is>
+      </c>
+      <c r="F6" s="4" t="n">
         <v>4</v>
       </c>
     </row>
     <row r="7" ht="14.3" customHeight="1">
       <c r="A7" s="1" t="n"/>
-      <c r="B7" s="3" t="inlineStr">
-        <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="C7" s="3" t="inlineStr">
-        <is>
-          <t>st</t>
-        </is>
-      </c>
-      <c r="D7" s="3" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="E7" s="4" t="inlineStr">
-        <is>
-          <t>st1</t>
-        </is>
-      </c>
-      <c r="F7" s="4" t="n">
+      <c r="E7" s="1" t="n">
+        <v>4</v>
+      </c>
+      <c r="F7" s="1" t="n">
         <v>5</v>
       </c>
     </row>
     <row r="8" ht="14.3" customHeight="1">
       <c r="A8" s="1" t="n"/>
-      <c r="B8" s="3" t="n"/>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="inlineStr">
+      <c r="B8" s="2" t="n"/>
+      <c r="C8" s="2" t="n"/>
+      <c r="D8" s="2" t="inlineStr">
         <is>
           <t>2.</t>
         </is>
       </c>
-      <c r="E8" s="4" t="inlineStr">
-        <is>
-          <t>st2</t>
-        </is>
-      </c>
-      <c r="F8" s="4" t="n">
+      <c r="E8" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="9" ht="14.3" customHeight="1">
       <c r="A9" s="1" t="n"/>
-      <c r="B9" s="2" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="C9" s="2" t="inlineStr">
-        <is>
-          <t>_0</t>
-        </is>
-      </c>
+      <c r="B9" s="2" t="n"/>
+      <c r="C9" s="2" t="n"/>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="E9" s="1" t="inlineStr">
-        <is>
-          <t>_01</t>
-        </is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="E9" s="1" t="n">
+        <v>7</v>
       </c>
       <c r="F9" s="1" t="n">
         <v>7</v>
@@ -672,35 +648,43 @@
     </row>
     <row r="10" ht="14.3" customHeight="1">
       <c r="A10" s="1" t="n"/>
-      <c r="B10" s="2" t="n"/>
-      <c r="C10" s="2" t="n"/>
-      <c r="D10" s="2" t="inlineStr">
-        <is>
-          <t>2.</t>
-        </is>
-      </c>
-      <c r="E10" s="1" t="inlineStr">
-        <is>
-          <t>_02</t>
-        </is>
-      </c>
-      <c r="F10" s="1" t="n">
+      <c r="B10" s="3" t="inlineStr">
+        <is>
+          <t>3.</t>
+        </is>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>10</v>
+      </c>
+      <c r="D10" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E10" s="4" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" s="4" t="n">
         <v>8</v>
       </c>
     </row>
     <row r="11" ht="14.3" customHeight="1">
       <c r="A11" s="1" t="n"/>
-      <c r="B11" s="2" t="n"/>
-      <c r="C11" s="2" t="n"/>
+      <c r="B11" s="2" t="inlineStr">
+        <is>
+          <t>4.</t>
+        </is>
+      </c>
+      <c r="C11" s="2" t="n">
+        <v>20</v>
+      </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>3.</t>
-        </is>
-      </c>
-      <c r="E11" s="1" t="inlineStr">
-        <is>
-          <t>_07</t>
-        </is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E11" s="1" t="n">
+        <v>22</v>
       </c>
       <c r="F11" s="1" t="n">
         <v>9</v>
@@ -708,57 +692,53 @@
     </row>
     <row r="12" ht="14.3" customHeight="1">
       <c r="A12" s="1" t="n"/>
-      <c r="B12" s="2" t="n"/>
-      <c r="C12" s="2" t="n"/>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>4.</t>
-        </is>
-      </c>
-      <c r="E12" s="1" t="inlineStr">
-        <is>
-          <t>_08</t>
-        </is>
-      </c>
-      <c r="F12" s="1" t="n">
+      <c r="B12" s="3" t="inlineStr">
+        <is>
+          <t>5.</t>
+        </is>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3" t="inlineStr">
+        <is>
+          <t>1.</t>
+        </is>
+      </c>
+      <c r="E12" s="4" t="n">
+        <v>105</v>
+      </c>
+      <c r="F12" s="4" t="n">
         <v>10</v>
       </c>
     </row>
     <row r="13" ht="14.3" customHeight="1">
       <c r="A13" s="1" t="n"/>
-      <c r="B13" s="2" t="n"/>
-      <c r="C13" s="2" t="n"/>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="E13" s="1" t="inlineStr">
-        <is>
-          <t>_09</t>
-        </is>
-      </c>
-      <c r="F13" s="1" t="n">
+      <c r="B13" s="3" t="n"/>
+      <c r="C13" s="3" t="n"/>
+      <c r="D13" s="3" t="inlineStr">
+        <is>
+          <t>2.</t>
+        </is>
+      </c>
+      <c r="E13" s="4" t="n">
+        <v>108</v>
+      </c>
+      <c r="F13" s="4" t="n">
         <v>11</v>
       </c>
     </row>
     <row r="14" ht="14.3" customHeight="1">
       <c r="A14" s="1" t="n"/>
-      <c r="B14" s="3" t="inlineStr">
-        <is>
-          <t>5.</t>
-        </is>
-      </c>
-      <c r="C14" s="3" t="n">
-        <v>1</v>
-      </c>
+      <c r="B14" s="3" t="n"/>
+      <c r="C14" s="3" t="n"/>
       <c r="D14" s="3" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>3.</t>
         </is>
       </c>
       <c r="E14" s="4" t="n">
-        <v>1</v>
+        <v>109</v>
       </c>
       <c r="F14" s="4" t="n">
         <v>12</v>
@@ -770,11 +750,11 @@
       <c r="C15" s="3" t="n"/>
       <c r="D15" s="3" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>4.</t>
         </is>
       </c>
       <c r="E15" s="4" t="n">
-        <v>2</v>
+        <v>117</v>
       </c>
       <c r="F15" s="4" t="n">
         <v>13</v>
@@ -786,11 +766,11 @@
       <c r="C16" s="3" t="n"/>
       <c r="D16" s="3" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>5.</t>
         </is>
       </c>
       <c r="E16" s="4" t="n">
-        <v>6</v>
+        <v>118</v>
       </c>
       <c r="F16" s="4" t="n">
         <v>14</v>
@@ -802,11 +782,11 @@
       <c r="C17" s="3" t="n"/>
       <c r="D17" s="3" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>6.</t>
         </is>
       </c>
       <c r="E17" s="4" t="n">
-        <v>7</v>
+        <v>119</v>
       </c>
       <c r="F17" s="4" t="n">
         <v>15</v>
@@ -814,193 +794,181 @@
     </row>
     <row r="18" ht="14.3" customHeight="1">
       <c r="A18" s="1" t="n"/>
-      <c r="B18" s="2" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="C18" s="2" t="n">
-        <v>10</v>
-      </c>
-      <c r="D18" s="2" t="inlineStr">
-        <is>
-          <t>1.</t>
-        </is>
-      </c>
-      <c r="E18" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="F18" s="1" t="n">
+      <c r="B18" s="3" t="n"/>
+      <c r="C18" s="3" t="n"/>
+      <c r="D18" s="3" t="inlineStr">
+        <is>
+          <t>7.</t>
+        </is>
+      </c>
+      <c r="E18" s="4" t="n">
+        <v>120</v>
+      </c>
+      <c r="F18" s="4" t="n">
         <v>16</v>
       </c>
     </row>
     <row r="19" ht="14.3" customHeight="1">
       <c r="A19" s="1" t="n"/>
-      <c r="B19" s="3" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="C19" s="3" t="n">
-        <v>100</v>
-      </c>
-      <c r="D19" s="3" t="inlineStr">
+      <c r="B19" s="2" t="inlineStr">
+        <is>
+          <t>6.</t>
+        </is>
+      </c>
+      <c r="C19" s="2" t="n">
+        <v>200</v>
+      </c>
+      <c r="D19" s="2" t="inlineStr">
         <is>
           <t>1.</t>
         </is>
       </c>
-      <c r="E19" s="4" t="n">
-        <v>101</v>
-      </c>
-      <c r="F19" s="4" t="n">
+      <c r="E19" s="1" t="n">
+        <v>201</v>
+      </c>
+      <c r="F19" s="1" t="n">
         <v>17</v>
       </c>
     </row>
     <row r="20" ht="14.3" customHeight="1">
       <c r="A20" s="1" t="n"/>
-      <c r="B20" s="3" t="n"/>
-      <c r="C20" s="3" t="n"/>
-      <c r="D20" s="3" t="inlineStr">
+      <c r="B20" s="2" t="n"/>
+      <c r="C20" s="2" t="n"/>
+      <c r="D20" s="2" t="inlineStr">
         <is>
           <t>2.</t>
         </is>
       </c>
-      <c r="E20" s="4" t="n">
-        <v>102</v>
-      </c>
-      <c r="F20" s="4" t="n">
+      <c r="E20" s="1" t="n">
+        <v>204</v>
+      </c>
+      <c r="F20" s="1" t="n">
         <v>18</v>
       </c>
     </row>
     <row r="21" ht="14.3" customHeight="1">
       <c r="A21" s="1" t="n"/>
-      <c r="B21" s="3" t="n"/>
-      <c r="C21" s="3" t="n"/>
-      <c r="D21" s="3" t="inlineStr">
+      <c r="B21" s="2" t="n"/>
+      <c r="C21" s="2" t="n"/>
+      <c r="D21" s="2" t="inlineStr">
         <is>
           <t>3.</t>
         </is>
       </c>
-      <c r="E21" s="4" t="n">
-        <v>103</v>
-      </c>
-      <c r="F21" s="4" t="n">
+      <c r="E21" s="1" t="n">
+        <v>206</v>
+      </c>
+      <c r="F21" s="1" t="n">
         <v>19</v>
       </c>
     </row>
     <row r="22" ht="14.3" customHeight="1">
       <c r="A22" s="1" t="n"/>
-      <c r="B22" s="3" t="n"/>
-      <c r="C22" s="3" t="n"/>
-      <c r="D22" s="3" t="inlineStr">
+      <c r="B22" s="2" t="n"/>
+      <c r="C22" s="2" t="n"/>
+      <c r="D22" s="2" t="inlineStr">
         <is>
           <t>4.</t>
         </is>
       </c>
-      <c r="E22" s="4" t="n">
-        <v>109</v>
-      </c>
-      <c r="F22" s="4" t="n">
+      <c r="E22" s="1" t="n">
+        <v>208</v>
+      </c>
+      <c r="F22" s="1" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="23" ht="14.3" customHeight="1">
       <c r="A23" s="1" t="n"/>
-      <c r="B23" s="3" t="n"/>
-      <c r="C23" s="3" t="n"/>
-      <c r="D23" s="3" t="inlineStr">
+      <c r="B23" s="2" t="n"/>
+      <c r="C23" s="2" t="n"/>
+      <c r="D23" s="2" t="inlineStr">
         <is>
           <t>5.</t>
         </is>
       </c>
-      <c r="E23" s="4" t="n">
-        <v>110</v>
-      </c>
-      <c r="F23" s="4" t="n">
+      <c r="E23" s="1" t="n">
+        <v>209</v>
+      </c>
+      <c r="F23" s="1" t="n">
         <v>21</v>
       </c>
     </row>
     <row r="24" ht="14.3" customHeight="1">
       <c r="A24" s="1" t="n"/>
-      <c r="B24" s="3" t="n"/>
-      <c r="C24" s="3" t="n"/>
-      <c r="D24" s="3" t="inlineStr">
+      <c r="B24" s="2" t="n"/>
+      <c r="C24" s="2" t="n"/>
+      <c r="D24" s="2" t="inlineStr">
         <is>
           <t>6.</t>
         </is>
       </c>
-      <c r="E24" s="4" t="n">
-        <v>111</v>
-      </c>
-      <c r="F24" s="4" t="n">
+      <c r="E24" s="1" t="n">
+        <v>212</v>
+      </c>
+      <c r="F24" s="1" t="n">
         <v>22</v>
       </c>
     </row>
     <row r="25" ht="14.3" customHeight="1">
       <c r="A25" s="1" t="n"/>
-      <c r="B25" s="3" t="n"/>
-      <c r="C25" s="3" t="n"/>
-      <c r="D25" s="3" t="inlineStr">
+      <c r="B25" s="2" t="n"/>
+      <c r="C25" s="2" t="n"/>
+      <c r="D25" s="2" t="inlineStr">
         <is>
           <t>7.</t>
         </is>
       </c>
-      <c r="E25" s="4" t="n">
-        <v>112</v>
-      </c>
-      <c r="F25" s="4" t="n">
+      <c r="E25" s="1" t="n">
+        <v>213</v>
+      </c>
+      <c r="F25" s="1" t="n">
         <v>23</v>
       </c>
     </row>
     <row r="26" ht="14.3" customHeight="1">
       <c r="A26" s="1" t="n"/>
-      <c r="B26" s="3" t="n"/>
-      <c r="C26" s="3" t="n"/>
-      <c r="D26" s="3" t="inlineStr">
+      <c r="B26" s="2" t="n"/>
+      <c r="C26" s="2" t="n"/>
+      <c r="D26" s="2" t="inlineStr">
         <is>
           <t>8.</t>
         </is>
       </c>
-      <c r="E26" s="4" t="n">
-        <v>115</v>
-      </c>
-      <c r="F26" s="4" t="n">
+      <c r="E26" s="1" t="n">
+        <v>216</v>
+      </c>
+      <c r="F26" s="1" t="n">
         <v>24</v>
       </c>
     </row>
     <row r="27" ht="14.3" customHeight="1">
       <c r="A27" s="1" t="n"/>
-      <c r="B27" s="3" t="n"/>
-      <c r="C27" s="3" t="n"/>
-      <c r="D27" s="3" t="inlineStr">
+      <c r="B27" s="2" t="n"/>
+      <c r="C27" s="2" t="n"/>
+      <c r="D27" s="2" t="inlineStr">
         <is>
           <t>9.</t>
         </is>
       </c>
-      <c r="E27" s="4" t="n">
-        <v>116</v>
-      </c>
-      <c r="F27" s="4" t="n">
+      <c r="E27" s="1" t="n">
+        <v>217</v>
+      </c>
+      <c r="F27" s="1" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="28" ht="14.3" customHeight="1">
       <c r="A28" s="1" t="n"/>
-      <c r="B28" s="2" t="inlineStr">
-        <is>
-          <t>8.</t>
-        </is>
-      </c>
-      <c r="C28" s="2" t="n">
-        <v>200</v>
-      </c>
+      <c r="B28" s="2" t="n"/>
+      <c r="C28" s="2" t="n"/>
       <c r="D28" s="2" t="inlineStr">
         <is>
-          <t>1.</t>
+          <t>10.</t>
         </is>
       </c>
       <c r="E28" s="1" t="n">
-        <v>201</v>
+        <v>218</v>
       </c>
       <c r="F28" s="1" t="n">
         <v>26</v>
@@ -1012,11 +980,11 @@
       <c r="C29" s="2" t="n"/>
       <c r="D29" s="2" t="inlineStr">
         <is>
-          <t>2.</t>
+          <t>11.</t>
         </is>
       </c>
       <c r="E29" s="1" t="n">
-        <v>202</v>
+        <v>219</v>
       </c>
       <c r="F29" s="1" t="n">
         <v>27</v>
@@ -1028,11 +996,11 @@
       <c r="C30" s="2" t="n"/>
       <c r="D30" s="2" t="inlineStr">
         <is>
-          <t>3.</t>
+          <t>12.</t>
         </is>
       </c>
       <c r="E30" s="1" t="n">
-        <v>203</v>
+        <v>220</v>
       </c>
       <c r="F30" s="1" t="n">
         <v>28</v>
@@ -1044,11 +1012,11 @@
       <c r="C31" s="2" t="n"/>
       <c r="D31" s="2" t="inlineStr">
         <is>
-          <t>4.</t>
+          <t>13.</t>
         </is>
       </c>
       <c r="E31" s="1" t="n">
-        <v>207</v>
+        <v>221</v>
       </c>
       <c r="F31" s="1" t="n">
         <v>29</v>
@@ -1060,62 +1028,26 @@
       <c r="C32" s="2" t="n"/>
       <c r="D32" s="2" t="inlineStr">
         <is>
-          <t>5.</t>
+          <t>14.</t>
         </is>
       </c>
       <c r="E32" s="1" t="n">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="F32" s="1" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="33" ht="14.3" customHeight="1">
-      <c r="A33" s="1" t="n"/>
-      <c r="B33" s="2" t="n"/>
-      <c r="C33" s="2" t="n"/>
-      <c r="D33" s="2" t="inlineStr">
-        <is>
-          <t>6.</t>
-        </is>
-      </c>
-      <c r="E33" s="1" t="n">
-        <v>209</v>
-      </c>
-      <c r="F33" s="1" t="n">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="34" ht="14.3" customHeight="1">
-      <c r="A34" s="1" t="n"/>
-      <c r="B34" s="2" t="n"/>
-      <c r="C34" s="2" t="n"/>
-      <c r="D34" s="2" t="inlineStr">
-        <is>
-          <t>7.</t>
-        </is>
-      </c>
-      <c r="E34" s="1" t="n">
-        <v>210</v>
-      </c>
-      <c r="F34" s="1" t="n">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="C9:C13"/>
-    <mergeCell ref="B14:B17"/>
-    <mergeCell ref="C14:C17"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B9:B13"/>
-    <mergeCell ref="C28:C34"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B28:B34"/>
-    <mergeCell ref="B19:B27"/>
-    <mergeCell ref="C19:C27"/>
-    <mergeCell ref="C4:C6"/>
+  <mergeCells count="8">
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="C12:C18"/>
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="B3:B6"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="B12:B18"/>
+    <mergeCell ref="B19:B32"/>
+    <mergeCell ref="C19:C32"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>